<commit_message>
Ejercicios de matrices 1-2-3-4
</commit_message>
<xml_diff>
--- a/Guia de Ejercicios Funciones Vectores Matrices/Ejercicio1/datos_prueba.xlsx
+++ b/Guia de Ejercicios Funciones Vectores Matrices/Ejercicio1/datos_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mabelo/CLionProjects/utnfrgpprogramacion2/Guia de Ejercicios Funciones Vectores Matrices/Ejercicio1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1589039F-8EE6-574F-BF27-2A9C1549F83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85940C89-92E2-8B4A-9E6A-661F5E17DE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{5D166FE8-4C9D-894C-B46B-4E571DC6B10F}"/>
   </bookViews>
@@ -36,15 +36,214 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+  <si>
+    <t>meto</t>
+  </si>
+  <si>
+    <t>saco</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <t>ultimo siempre queda</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF1C00CF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF1C00CF"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -67,8 +266,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,250 +583,553 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E111B0B-C0C8-FA4E-9CF4-F12425A496D7}">
-  <dimension ref="A1:A78"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>2</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="L23">
+        <v>6</v>
+      </c>
+      <c r="P23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3</v>
       </c>
@@ -783,6 +1286,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>